<commit_message>
Update last meeting main point, modify AI script
</commit_message>
<xml_diff>
--- a/assign03_meeting_diary.xlsx
+++ b/assign03_meeting_diary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cookd/teaching/ETC5521/eda-private/assignments/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/justinaight/Desktop/Monash/ETC5521 - Explanatory Data Analysis /assignment-3-dragon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44E6E8D6-D05B-C146-B3DA-2457C8448439}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B48F35A3-830F-4549-B213-889CBD934F89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7120" yWindow="820" windowWidth="27860" windowHeight="16940" xr2:uid="{AA36F377-8185-6045-958F-09DEEBD07722}"/>
+    <workbookView xWindow="940" yWindow="500" windowWidth="27860" windowHeight="16360" xr2:uid="{AA36F377-8185-6045-958F-09DEEBD07722}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Team Name:</t>
   </si>
@@ -61,9 +61,6 @@
   </si>
   <si>
     <t>Discussions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fill in as needed </t>
   </si>
   <si>
     <t>eg.
@@ -71,6 +68,28 @@
 Upload and populate the group diary
 Fix merge conflict 
 Decide on choice of methods for first part</t>
+  </si>
+  <si>
+    <t>dragon</t>
+  </si>
+  <si>
+    <t>vdoo0002</t>
+  </si>
+  <si>
+    <t>justin-git01</t>
+  </si>
+  <si>
+    <t>jsan0062</t>
+  </si>
+  <si>
+    <t>JaySangani</t>
+  </si>
+  <si>
+    <t>Proof-read on all tasks required
+Work allocated for each task
+Agree on deadline for submission on github of task 1
+Justin will fetch the data (Task2 and part of Task3) with help of Jay
+Post on ED if have any question</t>
   </si>
 </sst>
 </file>
@@ -141,7 +160,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,12 +478,13 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28.6640625" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" customWidth="1"/>
     <col min="5" max="5" width="38.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -472,11 +492,28 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
@@ -517,12 +554,24 @@
         <v>7</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="119" x14ac:dyDescent="0.2">
+      <c r="A8" s="7">
+        <v>45189</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.8125</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add meeting new tasks and deadline
</commit_message>
<xml_diff>
--- a/assign03_meeting_diary.xlsx
+++ b/assign03_meeting_diary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sem 2\Explonatory data analysis\assignment-3-dragon\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/justinaight/Desktop/Monash/ETC5521 - Explanatory Data Analysis /assignment-3-dragon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD4C0044-23E5-4BDA-AD44-035CC457DC3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C828D8-2FBA-7642-B3EA-5206660BB9B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{AA36F377-8185-6045-958F-09DEEBD07722}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25820" windowHeight="13900" xr2:uid="{AA36F377-8185-6045-958F-09DEEBD07722}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>Team Name:</t>
   </si>
@@ -81,6 +81,10 @@
 Agree on deadline for submission on github of task 1
 Justin will fetch the data (Task2 and part of Task3) with help of Jay
 Post on ED if have any question</t>
+  </si>
+  <si>
+    <t>Perform merging 
+divide workload for IDA part and set deadline</t>
   </si>
 </sst>
 </file>
@@ -466,20 +470,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B0CB73-A0EE-1845-ADEE-622320F90FF1}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28.6640625" customWidth="1"/>
     <col min="4" max="4" width="14.6640625" customWidth="1"/>
     <col min="5" max="5" width="38.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -487,7 +491,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -498,7 +502,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>13</v>
       </c>
@@ -506,15 +510,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -531,7 +535,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>45183</v>
       </c>
@@ -548,7 +552,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="108.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="119" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
         <v>45189</v>
       </c>
@@ -563,6 +567,23 @@
       </c>
       <c r="E8" s="6" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>45198</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finalise meeting diary and AI script
</commit_message>
<xml_diff>
--- a/assign03_meeting_diary.xlsx
+++ b/assign03_meeting_diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/justinaight/Desktop/Monash/ETC5521 - Explanatory Data Analysis /assignment-3-dragon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C828D8-2FBA-7642-B3EA-5206660BB9B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83F18624-0B98-0E4F-B454-4B97EA0A0309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25820" windowHeight="13900" xr2:uid="{AA36F377-8185-6045-958F-09DEEBD07722}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>Team Name:</t>
   </si>
@@ -85,6 +85,15 @@
   <si>
     <t>Perform merging 
 divide workload for IDA part and set deadline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All </t>
+  </si>
+  <si>
+    <t>Cross-checking IDA idea, and divide workload for EDA</t>
+  </si>
+  <si>
+    <t>Finalise every plot and graph, do the document and cross-check together</t>
   </si>
 </sst>
 </file>
@@ -143,7 +152,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -156,6 +165,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -470,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B0CB73-A0EE-1845-ADEE-622320F90FF1}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -586,6 +596,40 @@
         <v>16</v>
       </c>
     </row>
+    <row r="10" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>45203</v>
+      </c>
+      <c r="B10" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" s="8">
+        <v>45205</v>
+      </c>
+      <c r="B11" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.6875</v>
+      </c>
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Initial commit: add part 2 files
</commit_message>
<xml_diff>
--- a/assign03_meeting_diary.xlsx
+++ b/assign03_meeting_diary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/justinaight/Desktop/Monash/ETC5521 - Explanatory Data Analysis /assignment-3-dragon/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cookd/teaching/ETC5521/eda-private/assignments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83F18624-0B98-0E4F-B454-4B97EA0A0309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44E6E8D6-D05B-C146-B3DA-2457C8448439}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25820" windowHeight="13900" xr2:uid="{AA36F377-8185-6045-958F-09DEEBD07722}"/>
+    <workbookView xWindow="7120" yWindow="820" windowWidth="27860" windowHeight="16940" xr2:uid="{AA36F377-8185-6045-958F-09DEEBD07722}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,21 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Team Name:</t>
   </si>
@@ -52,6 +61,9 @@
   </si>
   <si>
     <t>Discussions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fill in as needed </t>
   </si>
   <si>
     <t>eg.
@@ -59,41 +71,6 @@
 Upload and populate the group diary
 Fix merge conflict 
 Decide on choice of methods for first part</t>
-  </si>
-  <si>
-    <t>dragon</t>
-  </si>
-  <si>
-    <t>vdoo0002</t>
-  </si>
-  <si>
-    <t>justin-git01</t>
-  </si>
-  <si>
-    <t>jsan0062</t>
-  </si>
-  <si>
-    <t>JaySangani</t>
-  </si>
-  <si>
-    <t>Proof-read on all tasks required
-Work allocated for each task
-Agree on deadline for submission on github of task 1
-Justin will fetch the data (Task2 and part of Task3) with help of Jay
-Post on ED if have any question</t>
-  </si>
-  <si>
-    <t>Perform merging 
-divide workload for IDA part and set deadline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">All </t>
-  </si>
-  <si>
-    <t>Cross-checking IDA idea, and divide workload for EDA</t>
-  </si>
-  <si>
-    <t>Finalise every plot and graph, do the document and cross-check together</t>
   </si>
 </sst>
 </file>
@@ -152,7 +129,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -164,8 +141,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -480,16 +456,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B0CB73-A0EE-1845-ADEE-622320F90FF1}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28.6640625" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" customWidth="1"/>
     <col min="5" max="5" width="38.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -497,28 +472,11 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
@@ -559,75 +517,12 @@
         <v>7</v>
       </c>
       <c r="E7" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="119" x14ac:dyDescent="0.2">
-      <c r="A8" s="7">
-        <v>45189</v>
-      </c>
-      <c r="B8" s="3">
-        <v>0.79166666666666663</v>
-      </c>
-      <c r="C8" s="3">
-        <v>0.8125</v>
-      </c>
-      <c r="D8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
-        <v>45198</v>
-      </c>
-      <c r="B9" s="3">
-        <v>0.45833333333333331</v>
-      </c>
-      <c r="C9" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="D9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
-        <v>45203</v>
-      </c>
-      <c r="B10" s="3">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="C10" s="3">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="D10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A11" s="8">
-        <v>45205</v>
-      </c>
-      <c r="B11" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="C11" s="3">
-        <v>0.6875</v>
-      </c>
-      <c r="D11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Team Diary and worked on Wrangling
</commit_message>
<xml_diff>
--- a/assign03_meeting_diary.xlsx
+++ b/assign03_meeting_diary.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJAY\exploratory data analysis\Assignment 3 part 2\assignment-3-dragon\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20927F1F-CDF5-402B-8B7C-41E122BBE434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>Team Name: Dragon</t>
   </si>
@@ -54,21 +63,39 @@
     <t>10/21/2023</t>
   </si>
   <si>
-    <t>Al</t>
-  </si>
-  <si>
     <t>Wrangled the sightings and tourism dataset</t>
+  </si>
+  <si>
+    <t>Attempted to Solve Wrangling Problems</t>
+  </si>
+  <si>
+    <t>Attempted to Solve Wrangling Problems + Attempted Temporal Analysis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Discussed fatal problems regarding wrangling and attempted to solve them </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="166" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Calibri"/>
@@ -76,24 +103,8 @@
     <font>
       <sz val="12"/>
       <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="15"/>
-      <color indexed="8"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -120,62 +131,53 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+  <cellXfs count="19">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="bottom"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="20" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -184,24 +186,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office Theme">
       <a:dk1>
@@ -403,7 +466,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -421,7 +484,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -450,7 +513,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -475,7 +538,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -500,7 +563,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -525,7 +588,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -550,7 +613,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -575,7 +638,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -600,7 +663,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -625,7 +688,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -650,7 +713,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -663,9 +726,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -682,7 +751,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -700,7 +769,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -725,7 +794,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -750,7 +819,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -775,7 +844,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -800,7 +869,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -825,7 +894,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -850,7 +919,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -875,7 +944,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -900,7 +969,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -925,7 +994,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -938,9 +1007,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -954,7 +1029,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -972,7 +1047,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1001,7 +1076,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1026,7 +1101,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1051,7 +1126,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1076,7 +1151,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1101,7 +1176,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1126,7 +1201,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1151,7 +1226,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1176,7 +1251,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1201,7 +1276,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1214,149 +1289,205 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.6719" style="1" customWidth="1"/>
-    <col min="2" max="4" width="11" style="1" customWidth="1"/>
-    <col min="5" max="5" width="38.3516" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="11" style="1" customWidth="1"/>
+    <col min="1" max="1" width="28.69921875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" style="1" customWidth="1"/>
+    <col min="5" max="5" width="65.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="17" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:5" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
     </row>
-    <row r="2" ht="17" customHeight="1">
-      <c r="A2" t="s" s="2">
+    <row r="2" spans="1:5" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
     </row>
-    <row r="3" ht="17" customHeight="1">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+    <row r="3" spans="1:5" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
     </row>
-    <row r="4" ht="17" customHeight="1">
-      <c r="A4" s="4"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+    <row r="4" spans="1:5" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="9"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
     </row>
-    <row r="5" ht="17" customHeight="1">
-      <c r="A5" t="s" s="2">
+    <row r="5" spans="1:5" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
     </row>
-    <row r="6" ht="17" customHeight="1">
-      <c r="A6" t="s" s="2">
+    <row r="6" spans="1:5" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B6" t="s" s="5">
+      <c r="B6" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C6" t="s" s="5">
+      <c r="C6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D6" t="s" s="5">
+      <c r="D6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E6" t="s" s="6">
+      <c r="E6" s="11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" ht="78.75" customHeight="1">
-      <c r="A7" s="7">
+    <row r="7" spans="1:5" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="12">
         <v>45214</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="13">
         <v>1.708333333333333</v>
       </c>
-      <c r="C7" s="8">
-        <v>1.722222222222222</v>
-      </c>
-      <c r="D7" t="s" s="9">
+      <c r="C7" s="13">
+        <v>1.7222222222222221</v>
+      </c>
+      <c r="D7" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E7" t="s" s="10">
+      <c r="E7" s="15" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" ht="17" customHeight="1">
-      <c r="A8" t="s" s="11">
+    <row r="8" spans="1:5" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="8">
-        <v>45221.875</v>
-      </c>
-      <c r="C8" s="8">
-        <v>45221.496527777781</v>
-      </c>
-      <c r="D8" t="s" s="9">
+      <c r="B8" s="13">
+        <v>1.75</v>
+      </c>
+      <c r="C8" s="13">
+        <v>0</v>
+      </c>
+      <c r="D8" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E8" t="s" s="9">
+      <c r="E8" s="14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" ht="17" customHeight="1">
-      <c r="A9" t="s" s="11">
+    <row r="9" spans="1:5" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="8">
-        <v>45221.916666666664</v>
-      </c>
-      <c r="C9" s="8">
-        <v>45221.496527777781</v>
-      </c>
-      <c r="D9" t="s" s="9">
+      <c r="B9" s="17">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C9" s="13">
+        <v>1.8055555555555554</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="E9" t="s" s="9">
+    </row>
+    <row r="10" spans="1:5" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>45222</v>
+      </c>
+      <c r="B10" s="13">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C10" s="13">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="18" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" ht="17" customHeight="1">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>45224</v>
+      </c>
+      <c r="B11" s="3">
+        <v>0.875</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.125</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>45225</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Added plots to check validity for regression
</commit_message>
<xml_diff>
--- a/assign03_meeting_diary.xlsx
+++ b/assign03_meeting_diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJAY\exploratory data analysis\Assignment 3 part 2\assignment-3-dragon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20927F1F-CDF5-402B-8B7C-41E122BBE434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{903861C9-1F27-456B-AB0D-A84F67BF34FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>Team Name: Dragon</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t xml:space="preserve">Discussed fatal problems regarding wrangling and attempted to solve them </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Discussion on how to conduct Regression Analysis and attempted for the same </t>
   </si>
 </sst>
 </file>
@@ -80,7 +83,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="h:mm;@"/>
+    <numFmt numFmtId="164" formatCode="h:mm;@"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -148,12 +151,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -168,7 +171,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -176,8 +179,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1308,10 +1312,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="A13" sqref="A13:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1485,6 +1489,23 @@
         <v>16</v>
       </c>
     </row>
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>45226</v>
+      </c>
+      <c r="B13" s="3">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
updated codes, added AI script and updated Team Diary
</commit_message>
<xml_diff>
--- a/assign03_meeting_diary.xlsx
+++ b/assign03_meeting_diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJAY\exploratory data analysis\Assignment 3 part 2\assignment-3-dragon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{903861C9-1F27-456B-AB0D-A84F67BF34FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A78A0796-6E5E-4A06-97B3-C15310473D93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t>Team Name: Dragon</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t xml:space="preserve">Discussion on how to conduct Regression Analysis and attempted for the same </t>
+  </si>
+  <si>
+    <t>Finished working on Regression and Created the presentation</t>
   </si>
 </sst>
 </file>
@@ -1312,10 +1315,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:E13"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1324,7 +1327,7 @@
     <col min="2" max="2" width="15.59765625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.59765625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="1" customWidth="1"/>
-    <col min="5" max="5" width="65.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="68.796875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" style="1" customWidth="1"/>
     <col min="7" max="16384" width="11" style="1"/>
   </cols>
@@ -1506,6 +1509,23 @@
         <v>17</v>
       </c>
     </row>
+    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>45227</v>
+      </c>
+      <c r="B14" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.8125</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>